<commit_message>
Formatting updates to buffer recipes
Moved title to header so it would populate across pages. Removed some of the recipes from "Western Blot Buffers" that were left over when the excel sheet was copied from "PhosTag Solutions" excel sheet
</commit_message>
<xml_diff>
--- a/Biochemistry/Solutions & Buffers/PhosTag_WesternBlot_BroadRange_Solutions/Western_blot_buffers.xlsx
+++ b/Biochemistry/Solutions & Buffers/PhosTag_WesternBlot_BroadRange_Solutions/Western_blot_buffers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinhunsucker/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Solutions &amp; Buffers\PhosTag_WesternBlot_BroadRange_Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C5F59B-323B-B646-B788-48C2661CAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05424752-0EC7-4E01-92F1-1976B6D278B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="29040" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,29 +18,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$C$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet3!$A$1:$D$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
   <si>
     <t>Compound</t>
   </si>
@@ -115,13 +102,7 @@
     <t>Amount for 100mL</t>
   </si>
   <si>
-    <t>20 mL</t>
-  </si>
-  <si>
     <t>D.I. H2O</t>
-  </si>
-  <si>
-    <t>80 mL</t>
   </si>
   <si>
     <t>Ponceau S</t>
@@ -232,18 +213,12 @@
   <si>
     <t>2L of Transfer Buffer (PTB) (2nd)</t>
   </si>
-  <si>
-    <t>100mL of Transfer Buffer + EDTA (3rd) (phostag only)</t>
-  </si>
-  <si>
-    <t>100mL of 20% Methanol (4th) (phostag only)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -286,13 +261,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -600,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -685,15 +653,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1015,32 +974,32 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.6640625" style="14"/>
+    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.7109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1060,25 +1019,25 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1061,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1071,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1122,9 +1081,9 @@
       <c r="C10" s="6"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>12</v>
@@ -1132,267 +1091,190 @@
       <c r="C11" s="9"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:4" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-    </row>
-    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+    </row>
+    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>13</v>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="21"/>
-    </row>
-    <row r="16" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-    </row>
-    <row r="19" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+    </row>
+    <row r="20" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-    </row>
-    <row r="24" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
+      <c r="B22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+    </row>
+    <row r="25" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="13"/>
-    </row>
-    <row r="27" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
     </row>
-    <row r="30" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="11" t="s">
-        <v>29</v>
+    <row r="31" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-    </row>
-    <row r="35" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-    </row>
-    <row r="40" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:3" ht="10.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A39:C39"/>
+  <mergeCells count="6">
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <firstHeader>&amp;LName:
-Date:&amp;C&amp;"Arial,Bold"&amp;18PhosTag Solutions</firstHeader>
+Date:&amp;C&amp;"Arial,Bold"&amp;18Western Blot Buffers</firstHeader>
   </headerFooter>
-  <rowBreaks count="3" manualBreakCount="3">
-    <brk id="17" max="3" man="1"/>
-    <brk id="33" max="16383" man="1"/>
-    <brk id="42" max="16383" man="1"/>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="23" max="16383" man="1"/>
+    <brk id="32" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -1409,26 +1291,26 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.6640625" style="14"/>
+    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.7109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1449,24 +1331,24 @@
       <c r="C3" s="6"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="4" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="29"/>
     </row>
-    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1477,16 +1359,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="25"/>
     </row>
-    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1495,33 +1377,33 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1532,30 +1414,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="13.35" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:C6"/>
@@ -1582,31 +1464,31 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.6640625" style="14"/>
+    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.7109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1620,7 +1502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1630,7 +1512,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1640,7 +1522,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1650,9 +1532,9 @@
       <c r="C5" s="6"/>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>12</v>
@@ -1660,15 +1542,15 @@
       <c r="C6" s="9"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1679,16 +1561,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1697,15 +1579,15 @@
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1716,46 +1598,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="11" t="s">
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
     </row>
-    <row r="20" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1766,33 +1648,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
     </row>
-    <row r="25" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1803,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -1812,24 +1694,24 @@
       </c>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
     </row>
-    <row r="30" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1840,16 +1722,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>17</v>
       </c>
@@ -1858,7 +1740,7 @@
       </c>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" ht="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="13.35" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A24:C24"/>
@@ -1881,21 +1763,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -2118,32 +1985,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A5D5A9-477B-4B97-9F9B-D797D2834A6C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2160,4 +2017,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Formatting updates to buffer recipes"
This reverts commit aa24d59ee9cdfa29ab4cd8088aa4abe8986ae17a.
</commit_message>
<xml_diff>
--- a/Biochemistry/Solutions & Buffers/PhosTag_WesternBlot_BroadRange_Solutions/Western_blot_buffers.xlsx
+++ b/Biochemistry/Solutions & Buffers/PhosTag_WesternBlot_BroadRange_Solutions/Western_blot_buffers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Solutions &amp; Buffers\PhosTag_WesternBlot_BroadRange_Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinhunsucker/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05424752-0EC7-4E01-92F1-1976B6D278B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C5F59B-323B-B646-B788-48C2661CAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="29040" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,29 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$C$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet3!$A$1:$D$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
   <si>
     <t>Compound</t>
   </si>
@@ -102,7 +115,13 @@
     <t>Amount for 100mL</t>
   </si>
   <si>
+    <t>20 mL</t>
+  </si>
+  <si>
     <t>D.I. H2O</t>
+  </si>
+  <si>
+    <t>80 mL</t>
   </si>
   <si>
     <t>Ponceau S</t>
@@ -213,12 +232,18 @@
   <si>
     <t>2L of Transfer Buffer (PTB) (2nd)</t>
   </si>
+  <si>
+    <t>100mL of Transfer Buffer + EDTA (3rd) (phostag only)</t>
+  </si>
+  <si>
+    <t>100mL of 20% Methanol (4th) (phostag only)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -261,6 +286,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -568,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +685,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -974,32 +1015,32 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.7109375" style="14"/>
+    <col min="5" max="5" width="14.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1019,25 +1060,25 @@
       </c>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="29"/>
     </row>
-    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1102,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1071,7 +1112,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -1081,9 +1122,9 @@
       <c r="C10" s="6"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>12</v>
@@ -1091,190 +1132,267 @@
       <c r="C11" s="9"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:4" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-    </row>
-    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+    </row>
+    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
+      <c r="B14" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+    </row>
+    <row r="19" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-    </row>
-    <row r="20" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="B26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="C26" s="13"/>
+    </row>
+    <row r="27" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:3" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-    </row>
-    <row r="25" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>16</v>
-      </c>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="10.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
     </row>
-    <row r="30" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>37</v>
+    <row r="31" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+    </row>
+    <row r="35" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="1:3" ht="10.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+    </row>
+    <row r="40" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" ht="10.35" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" ht="10.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <firstHeader>&amp;LName:
-Date:&amp;C&amp;"Arial,Bold"&amp;18Western Blot Buffers</firstHeader>
+Date:&amp;C&amp;"Arial,Bold"&amp;18PhosTag Solutions</firstHeader>
   </headerFooter>
-  <rowBreaks count="2" manualBreakCount="2">
-    <brk id="23" max="16383" man="1"/>
-    <brk id="32" max="16383" man="1"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="17" max="3" man="1"/>
+    <brk id="33" max="16383" man="1"/>
+    <brk id="42" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -1291,26 +1409,26 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.7109375" style="14"/>
+    <col min="5" max="5" width="14.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1331,24 +1449,24 @@
       <c r="C3" s="6"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="4" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="29"/>
     </row>
-    <row r="7" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1359,16 +1477,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="25"/>
     </row>
-    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1377,33 +1495,33 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1414,30 +1532,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="13.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A6:C6"/>
@@ -1464,31 +1582,31 @@
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.7109375" style="14"/>
+    <col min="5" max="5" width="14.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1512,7 +1630,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1522,7 +1640,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1532,9 +1650,9 @@
       <c r="C5" s="6"/>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>12</v>
@@ -1542,15 +1660,15 @@
       <c r="C6" s="9"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1561,16 +1679,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1579,15 +1697,15 @@
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1598,46 +1716,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="B17" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
     </row>
-    <row r="20" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1648,33 +1766,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="29"/>
     </row>
-    <row r="25" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -1694,24 +1812,24 @@
       </c>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
     </row>
-    <row r="30" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1722,16 +1840,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>17</v>
       </c>
@@ -1740,7 +1858,7 @@
       </c>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" ht="13.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A24:C24"/>
@@ -1763,6 +1881,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -1985,22 +2118,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A5D5A9-477B-4B97-9F9B-D797D2834A6C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2017,29 +2160,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>